<commit_message>
adding menu, start working on player editor
</commit_message>
<xml_diff>
--- a/ressources/tab/spell_tab.xlsx
+++ b/ressources/tab/spell_tab.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>PA</t>
   </si>
@@ -52,6 +52,63 @@
   </si>
   <si>
     <t>DIAM</t>
+  </si>
+  <si>
+    <t>7 8</t>
+  </si>
+  <si>
+    <t>8 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9 8</t>
+  </si>
+  <si>
+    <t>10 8</t>
+  </si>
+  <si>
+    <t>11 8</t>
+  </si>
+  <si>
+    <t>12 8</t>
+  </si>
+  <si>
+    <t>13 8</t>
+  </si>
+  <si>
+    <t>14 8</t>
+  </si>
+  <si>
+    <t>7 9</t>
+  </si>
+  <si>
+    <t>7 10</t>
+  </si>
+  <si>
+    <t>7 11</t>
+  </si>
+  <si>
+    <t>7 12</t>
+  </si>
+  <si>
+    <t>7 13</t>
+  </si>
+  <si>
+    <t>7 14</t>
+  </si>
+  <si>
+    <t>char 1</t>
+  </si>
+  <si>
+    <t>char 2</t>
+  </si>
+  <si>
+    <t>char 3</t>
+  </si>
+  <si>
+    <t>char 4</t>
+  </si>
+  <si>
+    <t>char 5</t>
   </si>
 </sst>
 </file>
@@ -441,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64:H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <f>B5+1</f>
+        <f t="shared" ref="B13:B19" si="19">B5+1</f>
         <v>1</v>
       </c>
       <c r="C13" s="7">
@@ -816,28 +873,28 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7">
-        <f t="shared" ref="G13" si="19">G$4*$A13+H$4*$B13</f>
+        <f t="shared" ref="G13" si="20">G$4*$A13+H$4*$B13</f>
         <v>2</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="7">
-        <f t="shared" ref="I13" si="20">I$4*$A13+J$4*$B13</f>
+        <f t="shared" ref="I13" si="21">I$4*$A13+J$4*$B13</f>
         <v>1</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="7">
-        <f t="shared" ref="K13" si="21">K$4*$A13+L$4*$B13</f>
+        <f t="shared" ref="K13" si="22">K$4*$A13+L$4*$B13</f>
         <v>1</v>
       </c>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f>MOD(A13 + 1, 7)</f>
+        <f t="shared" ref="A14:A19" si="23">MOD(A13 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B14">
-        <f>B6+1</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="C14" s="9">
@@ -851,28 +908,28 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="9">
-        <f t="shared" ref="G14" si="22">G$4*$A14+H$4*$B14</f>
+        <f t="shared" ref="G14" si="24">G$4*$A14+H$4*$B14</f>
         <v>4.25</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="9">
-        <f t="shared" ref="I14" si="23">I$4*$A14+J$4*$B14</f>
+        <f t="shared" ref="I14" si="25">I$4*$A14+J$4*$B14</f>
         <v>3</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="9">
-        <f t="shared" ref="K14" si="24">K$4*$A14+L$4*$B14</f>
+        <f t="shared" ref="K14" si="26">K$4*$A14+L$4*$B14</f>
         <v>2.85</v>
       </c>
       <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f>MOD(A14 + 1, 7)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="B15">
-        <f>B7+1</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="C15" s="9">
@@ -886,28 +943,28 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9">
-        <f t="shared" ref="G15" si="25">G$4*$A15+H$4*$B15</f>
+        <f t="shared" ref="G15" si="27">G$4*$A15+H$4*$B15</f>
         <v>6.5</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="9">
-        <f t="shared" ref="I15" si="26">I$4*$A15+J$4*$B15</f>
+        <f t="shared" ref="I15" si="28">I$4*$A15+J$4*$B15</f>
         <v>5</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="9">
-        <f t="shared" ref="K15" si="27">K$4*$A15+L$4*$B15</f>
+        <f t="shared" ref="K15" si="29">K$4*$A15+L$4*$B15</f>
         <v>4.7</v>
       </c>
       <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f>MOD(A15 + 1, 7)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="B16">
-        <f>B8+1</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="C16" s="9">
@@ -921,28 +978,28 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9">
-        <f t="shared" ref="G16" si="28">G$4*$A16+H$4*$B16</f>
+        <f t="shared" ref="G16" si="30">G$4*$A16+H$4*$B16</f>
         <v>8.75</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="9">
-        <f t="shared" ref="I16" si="29">I$4*$A16+J$4*$B16</f>
+        <f t="shared" ref="I16" si="31">I$4*$A16+J$4*$B16</f>
         <v>7</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="9">
-        <f t="shared" ref="K16" si="30">K$4*$A16+L$4*$B16</f>
+        <f t="shared" ref="K16" si="32">K$4*$A16+L$4*$B16</f>
         <v>6.5500000000000007</v>
       </c>
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f>MOD(A16 + 1, 7)</f>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="B17">
-        <f>B9+1</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="C17" s="9">
@@ -956,28 +1013,28 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="9">
-        <f t="shared" ref="G17" si="31">G$4*$A17+H$4*$B17</f>
+        <f t="shared" ref="G17" si="33">G$4*$A17+H$4*$B17</f>
         <v>11</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="9">
-        <f t="shared" ref="I17" si="32">I$4*$A17+J$4*$B17</f>
+        <f t="shared" ref="I17" si="34">I$4*$A17+J$4*$B17</f>
         <v>9</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="9">
-        <f t="shared" ref="K17" si="33">K$4*$A17+L$4*$B17</f>
+        <f t="shared" ref="K17" si="35">K$4*$A17+L$4*$B17</f>
         <v>8.4</v>
       </c>
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>MOD(A17 + 1, 7)</f>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="B18">
-        <f>B10+1</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="C18" s="9">
@@ -991,28 +1048,28 @@
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="9">
-        <f t="shared" ref="G18" si="34">G$4*$A18+H$4*$B18</f>
+        <f t="shared" ref="G18" si="36">G$4*$A18+H$4*$B18</f>
         <v>13.25</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="9">
-        <f t="shared" ref="I18" si="35">I$4*$A18+J$4*$B18</f>
+        <f t="shared" ref="I18" si="37">I$4*$A18+J$4*$B18</f>
         <v>11</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="9">
-        <f t="shared" ref="K18" si="36">K$4*$A18+L$4*$B18</f>
+        <f t="shared" ref="K18" si="38">K$4*$A18+L$4*$B18</f>
         <v>10.25</v>
       </c>
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>MOD(A18 + 1, 7)</f>
+        <f t="shared" si="23"/>
         <v>6</v>
       </c>
       <c r="B19">
-        <f>B11+1</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="C19" s="11">
@@ -1026,17 +1083,17 @@
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="11">
-        <f t="shared" ref="G19" si="37">G$4*$A19+H$4*$B19</f>
+        <f t="shared" ref="G19" si="39">G$4*$A19+H$4*$B19</f>
         <v>15.5</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="11">
-        <f t="shared" ref="I19" si="38">I$4*$A19+J$4*$B19</f>
+        <f t="shared" ref="I19" si="40">I$4*$A19+J$4*$B19</f>
         <v>13</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="11">
-        <f t="shared" ref="K19" si="39">K$4*$A19+L$4*$B19</f>
+        <f t="shared" ref="K19" si="41">K$4*$A19+L$4*$B19</f>
         <v>12.100000000000001</v>
       </c>
       <c r="L19" s="12"/>
@@ -1061,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <f>B13+1</f>
+        <f t="shared" ref="B21:B27" si="42">B13+1</f>
         <v>2</v>
       </c>
       <c r="C21" s="7">
@@ -1075,28 +1132,28 @@
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="7">
-        <f t="shared" ref="G21" si="40">G$4*$A21+H$4*$B21</f>
+        <f t="shared" ref="G21" si="43">G$4*$A21+H$4*$B21</f>
         <v>4</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="7">
-        <f t="shared" ref="I21" si="41">I$4*$A21+J$4*$B21</f>
+        <f t="shared" ref="I21" si="44">I$4*$A21+J$4*$B21</f>
         <v>2</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="7">
-        <f t="shared" ref="K21" si="42">K$4*$A21+L$4*$B21</f>
+        <f t="shared" ref="K21" si="45">K$4*$A21+L$4*$B21</f>
         <v>2</v>
       </c>
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f>MOD(A21 + 1, 7)</f>
+        <f t="shared" ref="A22:A27" si="46">MOD(A21 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B22">
-        <f>B14+1</f>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="C22" s="9">
@@ -1110,28 +1167,28 @@
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="9">
-        <f t="shared" ref="G22" si="43">G$4*$A22+H$4*$B22</f>
+        <f t="shared" ref="G22" si="47">G$4*$A22+H$4*$B22</f>
         <v>6.25</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="9">
-        <f t="shared" ref="I22" si="44">I$4*$A22+J$4*$B22</f>
+        <f t="shared" ref="I22" si="48">I$4*$A22+J$4*$B22</f>
         <v>4</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="9">
-        <f t="shared" ref="K22" si="45">K$4*$A22+L$4*$B22</f>
+        <f t="shared" ref="K22" si="49">K$4*$A22+L$4*$B22</f>
         <v>3.85</v>
       </c>
       <c r="L22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f>MOD(A22 + 1, 7)</f>
+        <f t="shared" si="46"/>
         <v>2</v>
       </c>
       <c r="B23">
-        <f>B15+1</f>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="C23" s="9">
@@ -1145,28 +1202,28 @@
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="9">
-        <f t="shared" ref="G23" si="46">G$4*$A23+H$4*$B23</f>
+        <f t="shared" ref="G23" si="50">G$4*$A23+H$4*$B23</f>
         <v>8.5</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="9">
-        <f t="shared" ref="I23" si="47">I$4*$A23+J$4*$B23</f>
+        <f t="shared" ref="I23" si="51">I$4*$A23+J$4*$B23</f>
         <v>6</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="9">
-        <f t="shared" ref="K23" si="48">K$4*$A23+L$4*$B23</f>
+        <f t="shared" ref="K23" si="52">K$4*$A23+L$4*$B23</f>
         <v>5.7</v>
       </c>
       <c r="L23" s="10"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f>MOD(A23 + 1, 7)</f>
+        <f t="shared" si="46"/>
         <v>3</v>
       </c>
       <c r="B24">
-        <f>B16+1</f>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="C24" s="9">
@@ -1180,28 +1237,28 @@
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="9">
-        <f t="shared" ref="G24" si="49">G$4*$A24+H$4*$B24</f>
+        <f t="shared" ref="G24" si="53">G$4*$A24+H$4*$B24</f>
         <v>10.75</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="9">
-        <f t="shared" ref="I24" si="50">I$4*$A24+J$4*$B24</f>
+        <f t="shared" ref="I24" si="54">I$4*$A24+J$4*$B24</f>
         <v>8</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="9">
-        <f t="shared" ref="K24" si="51">K$4*$A24+L$4*$B24</f>
+        <f t="shared" ref="K24" si="55">K$4*$A24+L$4*$B24</f>
         <v>7.5500000000000007</v>
       </c>
       <c r="L24" s="10"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f>MOD(A24 + 1, 7)</f>
+        <f t="shared" si="46"/>
         <v>4</v>
       </c>
       <c r="B25">
-        <f>B17+1</f>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="C25" s="9">
@@ -1215,28 +1272,28 @@
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="9">
-        <f t="shared" ref="G25" si="52">G$4*$A25+H$4*$B25</f>
+        <f t="shared" ref="G25" si="56">G$4*$A25+H$4*$B25</f>
         <v>13</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="9">
-        <f t="shared" ref="I25" si="53">I$4*$A25+J$4*$B25</f>
+        <f t="shared" ref="I25" si="57">I$4*$A25+J$4*$B25</f>
         <v>10</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="9">
-        <f t="shared" ref="K25" si="54">K$4*$A25+L$4*$B25</f>
+        <f t="shared" ref="K25" si="58">K$4*$A25+L$4*$B25</f>
         <v>9.4</v>
       </c>
       <c r="L25" s="10"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f>MOD(A25 + 1, 7)</f>
+        <f t="shared" si="46"/>
         <v>5</v>
       </c>
       <c r="B26">
-        <f>B18+1</f>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="C26" s="9">
@@ -1250,28 +1307,28 @@
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="9">
-        <f t="shared" ref="G26" si="55">G$4*$A26+H$4*$B26</f>
+        <f t="shared" ref="G26" si="59">G$4*$A26+H$4*$B26</f>
         <v>15.25</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="9">
-        <f t="shared" ref="I26" si="56">I$4*$A26+J$4*$B26</f>
+        <f t="shared" ref="I26" si="60">I$4*$A26+J$4*$B26</f>
         <v>12</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="9">
-        <f t="shared" ref="K26" si="57">K$4*$A26+L$4*$B26</f>
+        <f t="shared" ref="K26" si="61">K$4*$A26+L$4*$B26</f>
         <v>11.25</v>
       </c>
       <c r="L26" s="10"/>
     </row>
     <row r="27" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>MOD(A26 + 1, 7)</f>
+        <f t="shared" si="46"/>
         <v>6</v>
       </c>
       <c r="B27">
-        <f>B19+1</f>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="C27" s="11">
@@ -1285,17 +1342,17 @@
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="11">
-        <f t="shared" ref="G27" si="58">G$4*$A27+H$4*$B27</f>
+        <f t="shared" ref="G27" si="62">G$4*$A27+H$4*$B27</f>
         <v>17.5</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="11">
-        <f t="shared" ref="I27" si="59">I$4*$A27+J$4*$B27</f>
+        <f t="shared" ref="I27" si="63">I$4*$A27+J$4*$B27</f>
         <v>14</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="11">
-        <f t="shared" ref="K27" si="60">K$4*$A27+L$4*$B27</f>
+        <f t="shared" ref="K27" si="64">K$4*$A27+L$4*$B27</f>
         <v>13.100000000000001</v>
       </c>
       <c r="L27" s="12"/>
@@ -1321,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <f>B21+1</f>
+        <f t="shared" ref="B29:B35" si="65">B21+1</f>
         <v>3</v>
       </c>
       <c r="C29" s="7">
@@ -1335,28 +1392,28 @@
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="7">
-        <f t="shared" ref="G29" si="61">G$4*$A29+H$4*$B29</f>
+        <f t="shared" ref="G29" si="66">G$4*$A29+H$4*$B29</f>
         <v>6</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="7">
-        <f t="shared" ref="I29" si="62">I$4*$A29+J$4*$B29</f>
+        <f t="shared" ref="I29" si="67">I$4*$A29+J$4*$B29</f>
         <v>3</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="7">
-        <f t="shared" ref="K29" si="63">K$4*$A29+L$4*$B29</f>
+        <f t="shared" ref="K29" si="68">K$4*$A29+L$4*$B29</f>
         <v>3</v>
       </c>
       <c r="L29" s="8"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f>MOD(A29 + 1, 7)</f>
+        <f t="shared" ref="A30:A35" si="69">MOD(A29 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B30">
-        <f>B22+1</f>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="C30" s="9">
@@ -1370,28 +1427,28 @@
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="9">
-        <f t="shared" ref="G30" si="64">G$4*$A30+H$4*$B30</f>
+        <f t="shared" ref="G30" si="70">G$4*$A30+H$4*$B30</f>
         <v>8.25</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="9">
-        <f t="shared" ref="I30" si="65">I$4*$A30+J$4*$B30</f>
+        <f t="shared" ref="I30" si="71">I$4*$A30+J$4*$B30</f>
         <v>5</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="9">
-        <f t="shared" ref="K30" si="66">K$4*$A30+L$4*$B30</f>
+        <f t="shared" ref="K30" si="72">K$4*$A30+L$4*$B30</f>
         <v>4.8499999999999996</v>
       </c>
       <c r="L30" s="10"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f>MOD(A30 + 1, 7)</f>
+        <f t="shared" si="69"/>
         <v>2</v>
       </c>
       <c r="B31">
-        <f>B23+1</f>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="C31" s="9">
@@ -1405,28 +1462,28 @@
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="9">
-        <f t="shared" ref="G31" si="67">G$4*$A31+H$4*$B31</f>
+        <f t="shared" ref="G31" si="73">G$4*$A31+H$4*$B31</f>
         <v>10.5</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="9">
-        <f t="shared" ref="I31" si="68">I$4*$A31+J$4*$B31</f>
+        <f t="shared" ref="I31" si="74">I$4*$A31+J$4*$B31</f>
         <v>7</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="9">
-        <f t="shared" ref="K31" si="69">K$4*$A31+L$4*$B31</f>
+        <f t="shared" ref="K31" si="75">K$4*$A31+L$4*$B31</f>
         <v>6.7</v>
       </c>
       <c r="L31" s="10"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f>MOD(A31 + 1, 7)</f>
+        <f t="shared" si="69"/>
         <v>3</v>
       </c>
       <c r="B32">
-        <f>B24+1</f>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="C32" s="9">
@@ -1440,28 +1497,28 @@
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="9">
-        <f t="shared" ref="G32" si="70">G$4*$A32+H$4*$B32</f>
+        <f t="shared" ref="G32" si="76">G$4*$A32+H$4*$B32</f>
         <v>12.75</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="9">
-        <f t="shared" ref="I32" si="71">I$4*$A32+J$4*$B32</f>
+        <f t="shared" ref="I32" si="77">I$4*$A32+J$4*$B32</f>
         <v>9</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="9">
-        <f t="shared" ref="K32" si="72">K$4*$A32+L$4*$B32</f>
+        <f t="shared" ref="K32" si="78">K$4*$A32+L$4*$B32</f>
         <v>8.5500000000000007</v>
       </c>
       <c r="L32" s="10"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f>MOD(A32 + 1, 7)</f>
+        <f t="shared" si="69"/>
         <v>4</v>
       </c>
       <c r="B33">
-        <f>B25+1</f>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="C33" s="9">
@@ -1475,28 +1532,28 @@
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="9">
-        <f t="shared" ref="G33" si="73">G$4*$A33+H$4*$B33</f>
+        <f t="shared" ref="G33" si="79">G$4*$A33+H$4*$B33</f>
         <v>15</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="9">
-        <f t="shared" ref="I33" si="74">I$4*$A33+J$4*$B33</f>
+        <f t="shared" ref="I33" si="80">I$4*$A33+J$4*$B33</f>
         <v>11</v>
       </c>
       <c r="J33" s="10"/>
       <c r="K33" s="9">
-        <f t="shared" ref="K33" si="75">K$4*$A33+L$4*$B33</f>
+        <f t="shared" ref="K33" si="81">K$4*$A33+L$4*$B33</f>
         <v>10.4</v>
       </c>
       <c r="L33" s="10"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f>MOD(A33 + 1, 7)</f>
+        <f t="shared" si="69"/>
         <v>5</v>
       </c>
       <c r="B34">
-        <f>B26+1</f>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="C34" s="9">
@@ -1510,28 +1567,28 @@
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="9">
-        <f t="shared" ref="G34" si="76">G$4*$A34+H$4*$B34</f>
+        <f t="shared" ref="G34" si="82">G$4*$A34+H$4*$B34</f>
         <v>17.25</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="9">
-        <f t="shared" ref="I34" si="77">I$4*$A34+J$4*$B34</f>
+        <f t="shared" ref="I34" si="83">I$4*$A34+J$4*$B34</f>
         <v>13</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="9">
-        <f t="shared" ref="K34" si="78">K$4*$A34+L$4*$B34</f>
+        <f t="shared" ref="K34" si="84">K$4*$A34+L$4*$B34</f>
         <v>12.25</v>
       </c>
       <c r="L34" s="10"/>
     </row>
     <row r="35" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>MOD(A34 + 1, 7)</f>
+        <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="B35">
-        <f>B27+1</f>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="C35" s="11">
@@ -1545,17 +1602,17 @@
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="11">
-        <f t="shared" ref="G35" si="79">G$4*$A35+H$4*$B35</f>
+        <f t="shared" ref="G35" si="85">G$4*$A35+H$4*$B35</f>
         <v>19.5</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="11">
-        <f t="shared" ref="I35" si="80">I$4*$A35+J$4*$B35</f>
+        <f t="shared" ref="I35" si="86">I$4*$A35+J$4*$B35</f>
         <v>15</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="11">
-        <f t="shared" ref="K35" si="81">K$4*$A35+L$4*$B35</f>
+        <f t="shared" ref="K35" si="87">K$4*$A35+L$4*$B35</f>
         <v>14.100000000000001</v>
       </c>
       <c r="L35" s="12"/>
@@ -1580,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:B43" si="82">B29+1</f>
+        <f t="shared" ref="B37:B43" si="88">B29+1</f>
         <v>4</v>
       </c>
       <c r="C37" s="7">
@@ -1594,28 +1651,28 @@
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="7">
-        <f t="shared" ref="G37" si="83">G$4*$A37+H$4*$B37</f>
+        <f t="shared" ref="G37" si="89">G$4*$A37+H$4*$B37</f>
         <v>8</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="7">
-        <f t="shared" ref="I37" si="84">I$4*$A37+J$4*$B37</f>
+        <f t="shared" ref="I37" si="90">I$4*$A37+J$4*$B37</f>
         <v>4</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="7">
-        <f t="shared" ref="K37" si="85">K$4*$A37+L$4*$B37</f>
+        <f t="shared" ref="K37" si="91">K$4*$A37+L$4*$B37</f>
         <v>4</v>
       </c>
       <c r="L37" s="8"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
-        <f>MOD(A37 + 1, 7)</f>
+        <f t="shared" ref="A38:A43" si="92">MOD(A37 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B38">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>4</v>
       </c>
       <c r="C38" s="9">
@@ -1629,28 +1686,28 @@
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="9">
-        <f t="shared" ref="G38" si="86">G$4*$A38+H$4*$B38</f>
+        <f t="shared" ref="G38" si="93">G$4*$A38+H$4*$B38</f>
         <v>10.25</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="9">
-        <f t="shared" ref="I38" si="87">I$4*$A38+J$4*$B38</f>
+        <f t="shared" ref="I38" si="94">I$4*$A38+J$4*$B38</f>
         <v>6</v>
       </c>
       <c r="J38" s="10"/>
       <c r="K38" s="9">
-        <f t="shared" ref="K38" si="88">K$4*$A38+L$4*$B38</f>
+        <f t="shared" ref="K38" si="95">K$4*$A38+L$4*$B38</f>
         <v>5.85</v>
       </c>
       <c r="L38" s="10"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
-        <f>MOD(A38 + 1, 7)</f>
+        <f t="shared" si="92"/>
         <v>2</v>
       </c>
       <c r="B39">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>4</v>
       </c>
       <c r="C39" s="9">
@@ -1664,28 +1721,28 @@
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="9">
-        <f t="shared" ref="G39" si="89">G$4*$A39+H$4*$B39</f>
+        <f t="shared" ref="G39" si="96">G$4*$A39+H$4*$B39</f>
         <v>12.5</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="9">
-        <f t="shared" ref="I39" si="90">I$4*$A39+J$4*$B39</f>
+        <f t="shared" ref="I39" si="97">I$4*$A39+J$4*$B39</f>
         <v>8</v>
       </c>
       <c r="J39" s="10"/>
       <c r="K39" s="9">
-        <f t="shared" ref="K39" si="91">K$4*$A39+L$4*$B39</f>
+        <f t="shared" ref="K39" si="98">K$4*$A39+L$4*$B39</f>
         <v>7.7</v>
       </c>
       <c r="L39" s="10"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
-        <f>MOD(A39 + 1, 7)</f>
+        <f t="shared" si="92"/>
         <v>3</v>
       </c>
       <c r="B40">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>4</v>
       </c>
       <c r="C40" s="9">
@@ -1699,28 +1756,28 @@
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="9">
-        <f t="shared" ref="G40" si="92">G$4*$A40+H$4*$B40</f>
+        <f t="shared" ref="G40" si="99">G$4*$A40+H$4*$B40</f>
         <v>14.75</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="9">
-        <f t="shared" ref="I40" si="93">I$4*$A40+J$4*$B40</f>
+        <f t="shared" ref="I40" si="100">I$4*$A40+J$4*$B40</f>
         <v>10</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="9">
-        <f t="shared" ref="K40" si="94">K$4*$A40+L$4*$B40</f>
+        <f t="shared" ref="K40" si="101">K$4*$A40+L$4*$B40</f>
         <v>9.5500000000000007</v>
       </c>
       <c r="L40" s="10"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f>MOD(A40 + 1, 7)</f>
+        <f t="shared" si="92"/>
         <v>4</v>
       </c>
       <c r="B41">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>4</v>
       </c>
       <c r="C41" s="9">
@@ -1734,28 +1791,28 @@
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="9">
-        <f t="shared" ref="G41" si="95">G$4*$A41+H$4*$B41</f>
+        <f t="shared" ref="G41" si="102">G$4*$A41+H$4*$B41</f>
         <v>17</v>
       </c>
       <c r="H41" s="10"/>
       <c r="I41" s="9">
-        <f t="shared" ref="I41" si="96">I$4*$A41+J$4*$B41</f>
+        <f t="shared" ref="I41" si="103">I$4*$A41+J$4*$B41</f>
         <v>12</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="9">
-        <f t="shared" ref="K41" si="97">K$4*$A41+L$4*$B41</f>
+        <f t="shared" ref="K41" si="104">K$4*$A41+L$4*$B41</f>
         <v>11.4</v>
       </c>
       <c r="L41" s="10"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f>MOD(A41 + 1, 7)</f>
+        <f t="shared" si="92"/>
         <v>5</v>
       </c>
       <c r="B42">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>4</v>
       </c>
       <c r="C42" s="9">
@@ -1769,28 +1826,28 @@
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="9">
-        <f t="shared" ref="G42" si="98">G$4*$A42+H$4*$B42</f>
+        <f t="shared" ref="G42" si="105">G$4*$A42+H$4*$B42</f>
         <v>19.25</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="9">
-        <f t="shared" ref="I42" si="99">I$4*$A42+J$4*$B42</f>
+        <f t="shared" ref="I42" si="106">I$4*$A42+J$4*$B42</f>
         <v>14</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="9">
-        <f t="shared" ref="K42" si="100">K$4*$A42+L$4*$B42</f>
+        <f t="shared" ref="K42" si="107">K$4*$A42+L$4*$B42</f>
         <v>13.25</v>
       </c>
       <c r="L42" s="10"/>
     </row>
     <row r="43" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>MOD(A42 + 1, 7)</f>
+        <f t="shared" si="92"/>
         <v>6</v>
       </c>
       <c r="B43">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>4</v>
       </c>
       <c r="C43" s="11">
@@ -1804,22 +1861,170 @@
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="11">
-        <f t="shared" ref="G43" si="101">G$4*$A43+H$4*$B43</f>
+        <f t="shared" ref="G43" si="108">G$4*$A43+H$4*$B43</f>
         <v>21.5</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="11">
-        <f t="shared" ref="I43" si="102">I$4*$A43+J$4*$B43</f>
+        <f t="shared" ref="I43" si="109">I$4*$A43+J$4*$B43</f>
         <v>16</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="11">
-        <f t="shared" ref="K43" si="103">K$4*$A43+L$4*$B43</f>
+        <f t="shared" ref="K43" si="110">K$4*$A43+L$4*$B43</f>
         <v>15.100000000000001</v>
       </c>
       <c r="L43" s="12"/>
     </row>
     <row r="44" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57">
+        <v>250</v>
+      </c>
+      <c r="F57">
+        <v>40</v>
+      </c>
+      <c r="G57">
+        <v>20</v>
+      </c>
+      <c r="H57">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58">
+        <f>E57-E59-E60-E61-E62-E63</f>
+        <v>250</v>
+      </c>
+      <c r="F58">
+        <f t="shared" ref="F58:H58" si="111">F57-F59-F60-F61-F62-F63</f>
+        <v>40</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="111"/>
+        <v>20</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="111"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64">
+        <f>E63-E65-E66-E67-E68-E69</f>
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <f t="shared" ref="F64" si="112">F63-F65-F66-F67-F68-F69</f>
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <f t="shared" ref="G64" si="113">G63-G65-G66-G67-G68-G69</f>
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <f t="shared" ref="H64" si="114">H63-H65-H66-H67-H68-H69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2187,241 +2392,241 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <f>B5+1</f>
+        <f t="shared" ref="B13:B19" si="5">B5+1</f>
         <v>1</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" ref="C13:C19" si="5">C$4*$A13+D$4*$B13</f>
+        <f t="shared" ref="C13:C19" si="6">C$4*$A13+D$4*$B13</f>
         <v>2</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="7">
-        <f t="shared" ref="E13:E19" si="6">E$4*$A13+F$4*$B13</f>
+        <f t="shared" ref="E13:E19" si="7">E$4*$A13+F$4*$B13</f>
         <v>1</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7">
-        <f t="shared" ref="G13:G19" si="7">G$4*$A13+H$4*$B13</f>
+        <f t="shared" ref="G13:G19" si="8">G$4*$A13+H$4*$B13</f>
         <v>0.5</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="7">
-        <f t="shared" ref="I13:I19" si="8">I$4*$A13+J$4*$B13</f>
+        <f t="shared" ref="I13:I19" si="9">I$4*$A13+J$4*$B13</f>
         <v>0.5</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="7">
-        <f t="shared" ref="K13:K19" si="9">K$4*$A13+L$4*$B13</f>
+        <f t="shared" ref="K13:K19" si="10">K$4*$A13+L$4*$B13</f>
         <v>1</v>
       </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f>MOD(A13 + 1, 7)</f>
+        <f t="shared" ref="A14:A19" si="11">MOD(A13 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B14">
-        <f>B6+1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C14" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.75</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.25</v>
       </c>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f>MOD(A14 + 1, 7)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="B15">
-        <f>B7+1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C15" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.5</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.5</v>
       </c>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f>MOD(A15 + 1, 7)</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="B16">
-        <f>B8+1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C16" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.25</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.75</v>
       </c>
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f>MOD(A16 + 1, 7)</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="B17">
-        <f>B9+1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C17" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.5</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.5</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>MOD(A17 + 1, 7)</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="B18">
-        <f>B10+1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C18" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.5</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.75</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.25</v>
       </c>
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>MOD(A18 + 1, 7)</f>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="B19">
-        <f>B11+1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C19" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.5</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.5</v>
       </c>
       <c r="L19" s="5"/>
@@ -2445,241 +2650,241 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <f>B13+1</f>
+        <f t="shared" ref="B21:B27" si="12">B13+1</f>
         <v>2</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" ref="C21:C27" si="10">C$4*$A21+D$4*$B21</f>
+        <f t="shared" ref="C21:C27" si="13">C$4*$A21+D$4*$B21</f>
         <v>4</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="7">
-        <f t="shared" ref="E21:E27" si="11">E$4*$A21+F$4*$B21</f>
+        <f t="shared" ref="E21:E27" si="14">E$4*$A21+F$4*$B21</f>
         <v>2</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="7">
-        <f t="shared" ref="G21:G27" si="12">G$4*$A21+H$4*$B21</f>
+        <f t="shared" ref="G21:G27" si="15">G$4*$A21+H$4*$B21</f>
         <v>1</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="7">
-        <f t="shared" ref="I21:I27" si="13">I$4*$A21+J$4*$B21</f>
+        <f t="shared" ref="I21:I27" si="16">I$4*$A21+J$4*$B21</f>
         <v>1</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="7">
-        <f t="shared" ref="K21:K27" si="14">K$4*$A21+L$4*$B21</f>
+        <f t="shared" ref="K21:K27" si="17">K$4*$A21+L$4*$B21</f>
         <v>2</v>
       </c>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f>MOD(A21 + 1, 7)</f>
+        <f t="shared" ref="A22:A27" si="18">MOD(A21 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B22">
-        <f>B14+1</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C22" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>3.5</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>2.5</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>2.25</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.25</v>
       </c>
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f>MOD(A22 + 1, 7)</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="B23">
-        <f>B15+1</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C23" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>3.5</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>4.5</v>
       </c>
       <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f>MOD(A23 + 1, 7)</f>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="B24">
-        <f>B16+1</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C24" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>6.5</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>5.5</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>4.75</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>5.75</v>
       </c>
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f>MOD(A24 + 1, 7)</f>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="B25">
-        <f>B17+1</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C25" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>7</v>
       </c>
       <c r="L25" s="4"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f>MOD(A25 + 1, 7)</f>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="B26">
-        <f>B18+1</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C26" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>9.5</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>8.5</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>7.25</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>8.25</v>
       </c>
       <c r="L26" s="4"/>
     </row>
     <row r="27" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>MOD(A26 + 1, 7)</f>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="B27">
-        <f>B19+1</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C27" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8.5</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9.5</v>
       </c>
       <c r="L27" s="5"/>
@@ -2703,241 +2908,241 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <f>B21+1</f>
+        <f t="shared" ref="B29:B35" si="19">B21+1</f>
         <v>3</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" ref="C29:C35" si="15">C$4*$A29+D$4*$B29</f>
+        <f t="shared" ref="C29:C35" si="20">C$4*$A29+D$4*$B29</f>
         <v>6</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="7">
-        <f t="shared" ref="E29:E35" si="16">E$4*$A29+F$4*$B29</f>
+        <f t="shared" ref="E29:E35" si="21">E$4*$A29+F$4*$B29</f>
         <v>3</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="7">
-        <f t="shared" ref="G29:G35" si="17">G$4*$A29+H$4*$B29</f>
+        <f t="shared" ref="G29:G35" si="22">G$4*$A29+H$4*$B29</f>
         <v>1.5</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="7">
-        <f t="shared" ref="I29:I35" si="18">I$4*$A29+J$4*$B29</f>
+        <f t="shared" ref="I29:I35" si="23">I$4*$A29+J$4*$B29</f>
         <v>1.5</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="7">
-        <f t="shared" ref="K29:K35" si="19">K$4*$A29+L$4*$B29</f>
+        <f t="shared" ref="K29:K35" si="24">K$4*$A29+L$4*$B29</f>
         <v>3</v>
       </c>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f>MOD(A29 + 1, 7)</f>
+        <f t="shared" ref="A30:A35" si="25">MOD(A29 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B30">
-        <f>B22+1</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="C30" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>4.5</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>3</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>2.75</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>4.25</v>
       </c>
       <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f>MOD(A30 + 1, 7)</f>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="B31">
-        <f>B23+1</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="C31" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>6</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>4.5</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>5.5</v>
       </c>
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f>MOD(A31 + 1, 7)</f>
+        <f t="shared" si="25"/>
         <v>3</v>
       </c>
       <c r="B32">
-        <f>B24+1</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="C32" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>12</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>7.5</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>6</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>5.25</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>6.75</v>
       </c>
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f>MOD(A32 + 1, 7)</f>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="B33">
-        <f>B25+1</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="C33" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>14</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>7.5</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>6.5</v>
       </c>
       <c r="J33" s="10"/>
       <c r="K33" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f>MOD(A33 + 1, 7)</f>
+        <f t="shared" si="25"/>
         <v>5</v>
       </c>
       <c r="B34">
-        <f>B26+1</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="C34" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>10.5</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>9</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>7.75</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>9.25</v>
       </c>
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>MOD(A34 + 1, 7)</f>
+        <f t="shared" si="25"/>
         <v>6</v>
       </c>
       <c r="B35">
-        <f>B27+1</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="C35" s="11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>12</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10.5</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>9</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>10.5</v>
       </c>
       <c r="L35" s="5"/>
@@ -2961,241 +3166,241 @@
         <v>0</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:B43" si="20">B29+1</f>
+        <f t="shared" ref="B37:B43" si="26">B29+1</f>
         <v>4</v>
       </c>
       <c r="C37" s="7">
-        <f t="shared" ref="C37:C43" si="21">C$4*$A37+D$4*$B37</f>
+        <f t="shared" ref="C37:C43" si="27">C$4*$A37+D$4*$B37</f>
         <v>8</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="7">
-        <f t="shared" ref="E37:E43" si="22">E$4*$A37+F$4*$B37</f>
+        <f t="shared" ref="E37:E43" si="28">E$4*$A37+F$4*$B37</f>
         <v>4</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="7">
-        <f t="shared" ref="G37:G43" si="23">G$4*$A37+H$4*$B37</f>
+        <f t="shared" ref="G37:G43" si="29">G$4*$A37+H$4*$B37</f>
         <v>2</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="7">
-        <f t="shared" ref="I37:I43" si="24">I$4*$A37+J$4*$B37</f>
+        <f t="shared" ref="I37:I43" si="30">I$4*$A37+J$4*$B37</f>
         <v>2</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="7">
-        <f t="shared" ref="K37:K43" si="25">K$4*$A37+L$4*$B37</f>
+        <f t="shared" ref="K37:K43" si="31">K$4*$A37+L$4*$B37</f>
         <v>4</v>
       </c>
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
-        <f>MOD(A37 + 1, 7)</f>
+        <f t="shared" ref="A38:A43" si="32">MOD(A37 + 1, 7)</f>
         <v>1</v>
       </c>
       <c r="B38">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="C38" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>10</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>5.5</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>3.5</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>3.25</v>
       </c>
       <c r="J38" s="10"/>
       <c r="K38" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>5.25</v>
       </c>
       <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
-        <f>MOD(A38 + 1, 7)</f>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="B39">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="C39" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>12</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>7</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>5</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>4.5</v>
       </c>
       <c r="J39" s="10"/>
       <c r="K39" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>6.5</v>
       </c>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <f>MOD(A39 + 1, 7)</f>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="B40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="C40" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>8.5</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>6.5</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>5.75</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>7.75</v>
       </c>
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f>MOD(A40 + 1, 7)</f>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="B41">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="C41" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>16</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>8</v>
       </c>
       <c r="H41" s="10"/>
       <c r="I41" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>7</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f>MOD(A41 + 1, 7)</f>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="B42">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="C42" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>18</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>11.5</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>9.5</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>8.25</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>10.25</v>
       </c>
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>MOD(A42 + 1, 7)</f>
+        <f t="shared" si="32"/>
         <v>6</v>
       </c>
       <c r="B43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="C43" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>20</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="11">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>13</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>11</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>9.5</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>11.5</v>
       </c>
       <c r="L43" s="5"/>

</xml_diff>